<commit_message>
Multi Attribute SLA and Attribute based routing
</commit_message>
<xml_diff>
--- a/resources/excels/KE.xlsx
+++ b/resources/excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="34080" windowHeight="10080" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="34080" windowHeight="10080" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -208,6 +208,103 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rahul Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represent the customer Line type(Prepaid/postpaid/hybrid)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rahul Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rahul Gupta:
+This column represent the customer Type</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rahul Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represent customer service category</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rahul Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represent customer segment</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -266,12 +363,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rahul Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This column represent the customer Line type(Prepaid/postpaid/hybrid)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7899" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7901" uniqueCount="1365">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3628,9 +3749,6 @@
     <t>Airtel Money_Agent</t>
   </si>
   <si>
-    <t>100221003564</t>
-  </si>
-  <si>
     <t>110221003574</t>
   </si>
   <si>
@@ -4320,49 +4438,85 @@
     <t>Code</t>
   </si>
   <si>
+    <t>Customer Type</t>
+  </si>
+  <si>
+    <t>Service Category</t>
+  </si>
+  <si>
+    <t>Customer SubSegment</t>
+  </si>
+  <si>
+    <t>Interaction Channel</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Workgroup Name</t>
+  </si>
+  <si>
+    <t>Rule Priority</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Attribute name</t>
+  </si>
+  <si>
+    <t>Attribute value</t>
+  </si>
+  <si>
+    <t>lineType</t>
+  </si>
+  <si>
+    <t>customerVip</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Default SLA</t>
+  </si>
+  <si>
+    <t>customerSegment</t>
+  </si>
+  <si>
+    <t>VIP Consumer</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Premier with CRM</t>
+  </si>
+  <si>
+    <t>HYBRID</t>
+  </si>
+  <si>
     <t>VIP</t>
   </si>
   <si>
-    <t>Line Type</t>
-  </si>
-  <si>
-    <t>Customer Type</t>
-  </si>
-  <si>
-    <t>Service Category</t>
-  </si>
-  <si>
-    <t>Customer Segment</t>
-  </si>
-  <si>
-    <t>Customer SubSegment</t>
-  </si>
-  <si>
-    <t>Interaction Channel</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Workgroup Name</t>
-  </si>
-  <si>
-    <t>Rule Priority</t>
-  </si>
-  <si>
-    <t>Prepaid</t>
-  </si>
-  <si>
-    <t>Pre</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>Attribute name</t>
-  </si>
-  <si>
-    <t>Attribute value</t>
+    <t>customerType</t>
+  </si>
+  <si>
+    <t>serviceCategory</t>
+  </si>
+  <si>
+    <t>customerSubSegment</t>
+  </si>
+  <si>
+    <t>interactionChannel</t>
+  </si>
+  <si>
+    <t>ticketNumber</t>
+  </si>
+  <si>
+    <t>100721003079</t>
   </si>
 </sst>
 </file>
@@ -5475,8 +5629,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5531,10 +5685,10 @@
         <v>172</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>1248</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>1249</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -5542,7 +5696,7 @@
         <v>2394650</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>124</v>
@@ -5587,7 +5741,7 @@
         <v>789474747</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -5595,7 +5749,7 @@
         <v>2388192</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>123</v>
@@ -5644,7 +5798,7 @@
         <v>2394650</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>131</v>
@@ -5667,7 +5821,7 @@
         <v>789474747</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5675,7 +5829,7 @@
         <v>2388008</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>175</v>
@@ -5704,10 +5858,10 @@
         <v>13221514</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D6" s="98">
         <v>767240995</v>
@@ -8206,7 +8360,7 @@
         <v>113</v>
       </c>
       <c r="E1" s="98" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9465,7 +9619,7 @@
         <v>1019</v>
       </c>
       <c r="D53" s="89" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="E53" s="90" t="s">
         <v>84</v>
@@ -17196,7 +17350,7 @@
         <v>895</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C2" s="4">
         <v>4</v>
@@ -17211,7 +17365,7 @@
         <v>898</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>899</v>
@@ -17264,13 +17418,13 @@
         <v>911</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1255</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>1256</v>
-      </c>
       <c r="J1" s="99" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K1" s="4"/>
     </row>
@@ -17297,7 +17451,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -17306,10 +17460,10 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J3" s="100" t="b">
         <v>0</v>
@@ -17318,7 +17472,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="100" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B4" s="100"/>
       <c r="C4" s="100"/>
@@ -17335,7 +17489,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="100" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B5" s="100"/>
       <c r="C5" s="100"/>
@@ -17352,7 +17506,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="100" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B6" s="100"/>
       <c r="C6" s="100"/>
@@ -17369,7 +17523,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="100" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B7" s="100"/>
       <c r="C7" s="100"/>
@@ -17386,7 +17540,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="100" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B8" s="100"/>
       <c r="C8" s="100"/>
@@ -17403,7 +17557,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="100" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B9" s="100"/>
       <c r="C9" s="100"/>
@@ -17420,7 +17574,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="100" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B10" s="100"/>
       <c r="C10" s="100"/>
@@ -17437,7 +17591,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="100" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B11" s="100"/>
       <c r="C11" s="100"/>
@@ -17454,7 +17608,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="100" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B12" s="100"/>
       <c r="C12" s="100"/>
@@ -17471,7 +17625,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="100" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B13" s="100"/>
       <c r="C13" s="100"/>
@@ -17502,43 +17656,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="42.125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="54.875" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="29"/>
+    <col min="1" max="1" width="35.125" style="29" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.125" style="29" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.875" style="29" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="10.875" style="29" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>1289</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="39" t="s">
         <v>1290</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>1291</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>1292</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="C2" s="39" t="s">
         <v>1293</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>1295</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="39" t="s">
         <v>1296</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>1297</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -17546,125 +17700,125 @@
         <v>994</v>
       </c>
       <c r="B4" s="39" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>1298</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>1299</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>1300</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="C5" s="39" t="s">
         <v>1301</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>1303</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>1304</v>
       </c>
       <c r="C6" s="101"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>1305</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="C7" s="39" t="s">
         <v>1306</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>1307</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>1308</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="C8" s="39" t="s">
         <v>1309</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>1310</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>1311</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="C9" s="39" t="s">
         <v>1312</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>1314</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="C10" s="39" t="s">
         <v>1315</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B11" s="39" t="s">
         <v>1317</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="C11" s="39" t="s">
         <v>1318</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>1319</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B12" s="39" t="s">
         <v>1320</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="C12" s="39" t="s">
         <v>1321</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>1322</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>1323</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>1324</v>
       </c>
       <c r="C13" s="101"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B14" s="39" t="s">
         <v>1325</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>1326</v>
       </c>
       <c r="C14" s="101"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>1327</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="C15" s="39" t="s">
         <v>1328</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>1329</v>
       </c>
     </row>
   </sheetData>
@@ -18233,7 +18387,7 @@
         <v>876</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -18285,7 +18439,7 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="9.625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="13" max="13" width="12.375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -18323,10 +18477,10 @@
         <v>980</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1244</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
@@ -18334,7 +18488,7 @@
         <v>77</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>142</v>
@@ -18388,7 +18542,7 @@
         <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>148</v>
@@ -18436,7 +18590,7 @@
         <v>156</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -18555,7 +18709,7 @@
         <v>950</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>951</v>
@@ -18662,7 +18816,7 @@
         <v>975</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>148</v>
@@ -18777,19 +18931,19 @@
     </row>
     <row r="18" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B18" s="38" t="s">
         <v>1235</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="C18" s="38" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>1236</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="E18" s="38" t="s">
         <v>1257</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>1237</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>1258</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>902</v>
@@ -18804,67 +18958,67 @@
     </row>
     <row r="19" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C19" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D19" s="38" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>1239</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>1240</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="G19" s="38" t="s">
         <v>1241</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>1242</v>
       </c>
       <c r="H19" s="38" t="s">
         <v>144</v>
       </c>
       <c r="I19" s="95" t="s">
+        <v>1274</v>
+      </c>
+      <c r="J19" s="95" t="s">
         <v>1275</v>
       </c>
-      <c r="J19" s="95" t="s">
+      <c r="K19" s="95" t="s">
         <v>1276</v>
-      </c>
-      <c r="K19" s="95" t="s">
-        <v>1277</v>
       </c>
       <c r="L19" s="38" t="s">
         <v>145</v>
       </c>
       <c r="M19" s="38" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="N19" s="94"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1259</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1260</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D20" s="38" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E20" s="38" t="s">
         <v>1261</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="F20" s="38" t="s">
         <v>1262</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="G20" s="38" t="s">
         <v>1263</v>
-      </c>
-      <c r="G20" s="38" t="s">
-        <v>1264</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -18875,16 +19029,16 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>1331</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>1332</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>1333</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>992</v>
@@ -18893,16 +19047,16 @@
         <v>166</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>1334</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>1335</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>1336</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>1337</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -18920,8 +19074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18950,7 +19104,7 @@
     <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="26" width="23.875" customWidth="1" collapsed="1"/>
     <col min="27" max="27" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="54" width="11" style="4"/>
+    <col min="48" max="54" width="11" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19096,28 +19250,28 @@
         <v>43</v>
       </c>
       <c r="AV1" s="4" t="s">
-        <v>1339</v>
+        <v>1350</v>
       </c>
       <c r="AW1" s="4" t="s">
-        <v>1340</v>
+        <v>1349</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>1341</v>
+        <v>1359</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>1342</v>
+        <v>1360</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>1343</v>
+        <v>1353</v>
       </c>
       <c r="BA1" s="4" t="s">
-        <v>1344</v>
+        <v>1361</v>
       </c>
       <c r="BB1" s="4" t="s">
-        <v>1345</v>
+        <v>1362</v>
       </c>
       <c r="BC1" s="4" t="s">
-        <v>57</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="2" spans="1:55" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19186,13 +19340,23 @@
         <v>1</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>1350</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>1351</v>
-      </c>
+        <v>1357</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>1354</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="BB2"/>
       <c r="BC2" s="2" t="s">
-        <v>1110</v>
+        <v>1364</v>
       </c>
     </row>
   </sheetData>
@@ -19204,41 +19368,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="23.875" customWidth="1"/>
+    <col min="9" max="9" width="23.875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1338</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1339</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>1340</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="4" t="s">
         <v>1341</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1342</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1344</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1345</v>
       </c>
       <c r="I1" t="s">
         <v>74</v>
@@ -19267,13 +19432,16 @@
       <c r="Q1" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>1004</v>
+        <v>1351</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -19282,7 +19450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -19293,10 +19461,13 @@
         <v>3</v>
       </c>
       <c r="Q3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -19310,10 +19481,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
+      <c r="B5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>1346</v>
+      </c>
       <c r="I5" t="s">
         <v>1004</v>
       </c>
@@ -19321,10 +19502,10 @@
         <v>3</v>
       </c>
       <c r="Q5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -19338,7 +19519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -19352,7 +19533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -19366,7 +19547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -19382,7 +19563,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19390,29 +19572,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.125" customWidth="1"/>
-    <col min="5" max="5" width="17.375" customWidth="1"/>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B1" t="s">
-        <v>1352</v>
+        <v>1347</v>
       </c>
       <c r="C1" t="s">
-        <v>1353</v>
+        <v>1348</v>
       </c>
       <c r="D1" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="E1" t="s">
         <v>86</v>
@@ -19421,10 +19603,10 @@
         <v>87</v>
       </c>
       <c r="G1" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="H1" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -19432,7 +19614,10 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>1339</v>
+        <v>1350</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1004</v>
@@ -19447,18 +19632,21 @@
         <v>114</v>
       </c>
       <c r="H2">
-        <v>-1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>1349</v>
+      </c>
       <c r="C3" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -19469,10 +19657,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19518,23 +19706,6 @@
       </c>
       <c r="E2" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -19823,7 +19994,7 @@
         <v>89</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="3" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -19910,7 +20081,7 @@
         <v>89</v>
       </c>
       <c r="BG3" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="4" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -19991,7 +20162,7 @@
         <v>89</v>
       </c>
       <c r="BG4" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="5" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20078,7 +20249,7 @@
         <v>89</v>
       </c>
       <c r="BG5" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -20153,7 +20324,7 @@
         <v>89</v>
       </c>
       <c r="BG6" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="7" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20303,7 +20474,7 @@
         <v>89</v>
       </c>
       <c r="BG8" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20378,7 +20549,7 @@
         <v>89</v>
       </c>
       <c r="BG9" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="10" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -20465,7 +20636,7 @@
         <v>89</v>
       </c>
       <c r="BG10" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="11" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -20528,7 +20699,7 @@
         <v>89</v>
       </c>
       <c r="BG11" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="12" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20603,7 +20774,7 @@
         <v>89</v>
       </c>
       <c r="BG12" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="13" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20678,7 +20849,7 @@
         <v>89</v>
       </c>
       <c r="BG13" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="14" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -20753,7 +20924,7 @@
         <v>89</v>
       </c>
       <c r="BG14" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="15" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20834,7 +21005,7 @@
         <v>89</v>
       </c>
       <c r="BG15" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="16" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20897,7 +21068,7 @@
         <v>89</v>
       </c>
       <c r="BG16" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="17" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -20960,7 +21131,7 @@
         <v>89</v>
       </c>
       <c r="BG17" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="18" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -21108,7 +21279,7 @@
         <v>89</v>
       </c>
       <c r="BG19" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
@@ -21201,7 +21372,7 @@
         <v>89</v>
       </c>
       <c r="BG20" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
@@ -21294,7 +21465,7 @@
         <v>89</v>
       </c>
       <c r="BG21" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
@@ -21387,7 +21558,7 @@
         <v>89</v>
       </c>
       <c r="BG22" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -21480,7 +21651,7 @@
         <v>89</v>
       </c>
       <c r="BG23" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -21573,7 +21744,7 @@
         <v>89</v>
       </c>
       <c r="BG24" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -21666,7 +21837,7 @@
         <v>89</v>
       </c>
       <c r="BG25" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -21765,7 +21936,7 @@
         <v>89</v>
       </c>
       <c r="BG26" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="27" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -21913,7 +22084,7 @@
         <v>89</v>
       </c>
       <c r="BG28" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="29" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21976,7 +22147,7 @@
         <v>89</v>
       </c>
       <c r="BG29" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="30" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -22039,7 +22210,7 @@
         <v>89</v>
       </c>
       <c r="BG30" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="31" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -22102,7 +22273,7 @@
         <v>89</v>
       </c>
       <c r="BG31" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="32" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -22165,7 +22336,7 @@
         <v>89</v>
       </c>
       <c r="BG32" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="33" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -22228,7 +22399,7 @@
         <v>89</v>
       </c>
       <c r="BG33" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="34" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -22315,7 +22486,7 @@
         <v>89</v>
       </c>
       <c r="BG34" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="35" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -22408,7 +22579,7 @@
         <v>89</v>
       </c>
       <c r="BG35" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="36" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -22489,7 +22660,7 @@
         <v>89</v>
       </c>
       <c r="BG36" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="37" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -22564,7 +22735,7 @@
         <v>89</v>
       </c>
       <c r="BG37" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="38" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -22639,7 +22810,7 @@
         <v>89</v>
       </c>
       <c r="BG38" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="39" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -22714,7 +22885,7 @@
         <v>89</v>
       </c>
       <c r="BG39" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="40" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -22801,7 +22972,7 @@
         <v>89</v>
       </c>
       <c r="BG40" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="41" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -22888,7 +23059,7 @@
         <v>89</v>
       </c>
       <c r="BG41" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="42" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -22951,7 +23122,7 @@
         <v>89</v>
       </c>
       <c r="BG42" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="43" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -23020,7 +23191,7 @@
         <v>89</v>
       </c>
       <c r="BG43" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="44" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23083,7 +23254,7 @@
         <v>89</v>
       </c>
       <c r="BG44" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="45" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -23146,7 +23317,7 @@
         <v>89</v>
       </c>
       <c r="BG45" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="46" spans="1:59" ht="102" x14ac:dyDescent="0.25">
@@ -23207,7 +23378,7 @@
         <v>89</v>
       </c>
       <c r="BG46" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="47" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -23282,7 +23453,7 @@
         <v>89</v>
       </c>
       <c r="BG47" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="48" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -23345,7 +23516,7 @@
         <v>89</v>
       </c>
       <c r="BG48" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="49" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23420,7 +23591,7 @@
         <v>89</v>
       </c>
       <c r="BG49" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="50" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -23495,7 +23666,7 @@
         <v>89</v>
       </c>
       <c r="BG50" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="51" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -23570,7 +23741,7 @@
         <v>89</v>
       </c>
       <c r="BG51" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="52" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -23645,7 +23816,7 @@
         <v>89</v>
       </c>
       <c r="BG52" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="53" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -23708,7 +23879,7 @@
         <v>89</v>
       </c>
       <c r="BG53" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="54" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -23777,7 +23948,7 @@
         <v>89</v>
       </c>
       <c r="BG54" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="55" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -23864,7 +24035,7 @@
         <v>89</v>
       </c>
       <c r="BG55" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="56" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -23927,7 +24098,7 @@
         <v>89</v>
       </c>
       <c r="BG56" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="57" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23990,7 +24161,7 @@
         <v>89</v>
       </c>
       <c r="BG57" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="58" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24065,7 +24236,7 @@
         <v>89</v>
       </c>
       <c r="BG58" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="59" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -24146,7 +24317,7 @@
         <v>89</v>
       </c>
       <c r="BG59" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="60" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -24227,7 +24398,7 @@
         <v>89</v>
       </c>
       <c r="BG60" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="61" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24290,7 +24461,7 @@
         <v>89</v>
       </c>
       <c r="BG61" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="62" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24353,7 +24524,7 @@
         <v>89</v>
       </c>
       <c r="BG62" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="63" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24416,7 +24587,7 @@
         <v>89</v>
       </c>
       <c r="BG63" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="64" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24479,7 +24650,7 @@
         <v>89</v>
       </c>
       <c r="BG64" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="65" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24554,7 +24725,7 @@
         <v>89</v>
       </c>
       <c r="BG65" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="66" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24623,7 +24794,7 @@
         <v>89</v>
       </c>
       <c r="BG66" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="67" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24698,7 +24869,7 @@
         <v>89</v>
       </c>
       <c r="BG67" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="68" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24761,7 +24932,7 @@
         <v>89</v>
       </c>
       <c r="BG68" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="69" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24836,7 +25007,7 @@
         <v>89</v>
       </c>
       <c r="BG69" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="70" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24911,7 +25082,7 @@
         <v>89</v>
       </c>
       <c r="BG70" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="71" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24974,7 +25145,7 @@
         <v>89</v>
       </c>
       <c r="BG71" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="72" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25043,7 +25214,7 @@
         <v>89</v>
       </c>
       <c r="BG72" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -25112,7 +25283,7 @@
         <v>89</v>
       </c>
       <c r="BG73" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -25187,7 +25358,7 @@
         <v>89</v>
       </c>
       <c r="BG74" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="75" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -25262,7 +25433,7 @@
         <v>89</v>
       </c>
       <c r="BG75" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="76" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25325,7 +25496,7 @@
         <v>89</v>
       </c>
       <c r="BG76" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="77" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -25388,7 +25559,7 @@
         <v>89</v>
       </c>
       <c r="BG77" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="78" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25451,7 +25622,7 @@
         <v>89</v>
       </c>
       <c r="BG78" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="79" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25526,7 +25697,7 @@
         <v>89</v>
       </c>
       <c r="BG79" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="80" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25589,7 +25760,7 @@
         <v>89</v>
       </c>
       <c r="BG80" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="81" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -25658,7 +25829,7 @@
         <v>89</v>
       </c>
       <c r="BG81" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="82" spans="1:59" x14ac:dyDescent="0.25">
@@ -25757,7 +25928,7 @@
         <v>89</v>
       </c>
       <c r="BG82" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="83" spans="1:59" x14ac:dyDescent="0.25">
@@ -25856,7 +26027,7 @@
         <v>89</v>
       </c>
       <c r="BG83" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="84" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -25919,7 +26090,7 @@
         <v>89</v>
       </c>
       <c r="BG84" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="85" spans="1:59" x14ac:dyDescent="0.25">
@@ -26012,7 +26183,7 @@
         <v>89</v>
       </c>
       <c r="BG85" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="86" spans="1:59" x14ac:dyDescent="0.25">
@@ -26105,7 +26276,7 @@
         <v>89</v>
       </c>
       <c r="BG86" s="1" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="87" spans="1:59" x14ac:dyDescent="0.25">
@@ -26204,7 +26375,7 @@
         <v>89</v>
       </c>
       <c r="BG87" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="88" spans="1:59" x14ac:dyDescent="0.25">
@@ -26297,7 +26468,7 @@
         <v>89</v>
       </c>
       <c r="BG88" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="89" spans="1:59" x14ac:dyDescent="0.25">
@@ -26396,7 +26567,7 @@
         <v>89</v>
       </c>
       <c r="BG89" s="1" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="90" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -26489,7 +26660,7 @@
         <v>89</v>
       </c>
       <c r="BG90" s="1" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="91" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -26564,7 +26735,7 @@
         <v>89</v>
       </c>
       <c r="BG91" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="92" spans="1:59" x14ac:dyDescent="0.25">
@@ -26639,7 +26810,7 @@
         <v>89</v>
       </c>
       <c r="BG92" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="93" spans="1:59" x14ac:dyDescent="0.25">
@@ -26714,7 +26885,7 @@
         <v>89</v>
       </c>
       <c r="BG93" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="94" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -26777,7 +26948,7 @@
         <v>89</v>
       </c>
       <c r="BG94" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="95" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -26840,7 +27011,7 @@
         <v>89</v>
       </c>
       <c r="BG95" s="1" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="96" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -26903,7 +27074,7 @@
         <v>89</v>
       </c>
       <c r="BG96" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="97" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -26966,7 +27137,7 @@
         <v>89</v>
       </c>
       <c r="BG97" s="1" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="98" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27029,7 +27200,7 @@
         <v>89</v>
       </c>
       <c r="BG98" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="99" spans="1:59" ht="102" x14ac:dyDescent="0.25">
@@ -27092,7 +27263,7 @@
         <v>89</v>
       </c>
       <c r="BG99" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="100" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -27167,7 +27338,7 @@
         <v>89</v>
       </c>
       <c r="BG100" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="101" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -27242,7 +27413,7 @@
         <v>89</v>
       </c>
       <c r="BG101" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="102" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -27317,7 +27488,7 @@
         <v>89</v>
       </c>
       <c r="BG102" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="103" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -27404,7 +27575,7 @@
         <v>89</v>
       </c>
       <c r="BG103" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.25">
@@ -27485,7 +27656,7 @@
         <v>89</v>
       </c>
       <c r="BG104" s="40" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="105" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27560,7 +27731,7 @@
         <v>89</v>
       </c>
       <c r="BG105" s="1" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="106" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27635,7 +27806,7 @@
         <v>89</v>
       </c>
       <c r="BG106" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="107" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27710,7 +27881,7 @@
         <v>89</v>
       </c>
       <c r="BG107" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="108" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27785,7 +27956,7 @@
         <v>89</v>
       </c>
       <c r="BG108" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="109" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -27860,7 +28031,7 @@
         <v>89</v>
       </c>
       <c r="BG109" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="110" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -27935,7 +28106,7 @@
         <v>89</v>
       </c>
       <c r="BG110" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="111" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -28016,7 +28187,7 @@
         <v>89</v>
       </c>
       <c r="BG111" s="1" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="112" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -28109,7 +28280,7 @@
         <v>89</v>
       </c>
       <c r="BG112" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="113" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -28196,7 +28367,7 @@
         <v>89</v>
       </c>
       <c r="BG113" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="114" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -28265,7 +28436,7 @@
         <v>89</v>
       </c>
       <c r="BG114" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="115" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -28358,7 +28529,7 @@
         <v>89</v>
       </c>
       <c r="BG115" s="1" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="116" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -28451,7 +28622,7 @@
         <v>89</v>
       </c>
       <c r="BG116" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="117" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -28544,7 +28715,7 @@
         <v>89</v>
       </c>
       <c r="BG117" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="118" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -28607,7 +28778,7 @@
         <v>89</v>
       </c>
       <c r="BG118" s="1" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="119" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -28688,7 +28859,7 @@
         <v>89</v>
       </c>
       <c r="BG119" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="120" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -28775,7 +28946,7 @@
         <v>89</v>
       </c>
       <c r="BG120" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="121" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -28862,7 +29033,7 @@
         <v>89</v>
       </c>
       <c r="BG121" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="122" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -28925,7 +29096,7 @@
         <v>89</v>
       </c>
       <c r="BG122" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="123" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -28988,7 +29159,7 @@
         <v>89</v>
       </c>
       <c r="BG123" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="124" spans="1:59" ht="127.5" x14ac:dyDescent="0.25">
@@ -29051,7 +29222,7 @@
         <v>89</v>
       </c>
       <c r="BG124" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="125" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -29138,7 +29309,7 @@
         <v>89</v>
       </c>
       <c r="BG125" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="126" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -29225,7 +29396,7 @@
         <v>89</v>
       </c>
       <c r="BG126" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="127" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -29470,7 +29641,7 @@
         <v>89</v>
       </c>
       <c r="BG129" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="130" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -29545,7 +29716,7 @@
         <v>89</v>
       </c>
       <c r="BG130" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes added for linked msisdn to account number
</commit_message>
<xml_diff>
--- a/resources/excels/KE.xlsx
+++ b/resources/excels/KE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lt13221390/Documents/Customer-portal/cs-portal-automation_selenium/resources/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFD3052-E0B5-3A4B-805E-1BF096935E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA96D9-37DB-F54B-A9EA-6F619230FCF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34080" windowHeight="10080" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8670" uniqueCount="1253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8682" uniqueCount="1263">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -4289,6 +4289,36 @@
   </si>
   <si>
     <t>Actions</t>
+  </si>
+  <si>
+    <t>LINKED MSISDN</t>
+  </si>
+  <si>
+    <t>MSISDN</t>
+  </si>
+  <si>
+    <t>SIM Number</t>
+  </si>
+  <si>
+    <t>GSM Service Activation Date</t>
+  </si>
+  <si>
+    <t>Line Type</t>
+  </si>
+  <si>
+    <t>Payment Level</t>
+  </si>
+  <si>
+    <t>GSM Status</t>
+  </si>
+  <si>
+    <t>Current Usage Limit</t>
+  </si>
+  <si>
+    <t>CUG</t>
+  </si>
+  <si>
+    <t>Security Deposit</t>
   </si>
 </sst>
 </file>
@@ -4491,7 +4521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -4586,6 +4616,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4603,7 +4642,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -4770,6 +4809,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18288,10 +18328,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -19003,6 +19043,44 @@
       </c>
       <c r="H24" s="98" t="s">
         <v>1252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="103" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B25" s="98" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C25" s="98" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D25" s="98" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E25" s="98" t="s">
+        <v>1257</v>
+      </c>
+      <c r="F25" s="98" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G25" s="104" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H25" s="104" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I25" s="104" t="s">
+        <v>1230</v>
+      </c>
+      <c r="J25" s="104" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K25" s="104" t="s">
+        <v>99</v>
+      </c>
+      <c r="L25" s="104" t="s">
+        <v>1262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes added for 1.11 & 1.12 prod issues
</commit_message>
<xml_diff>
--- a/resources/excels/KE.xlsx
+++ b/resources/excels/KE.xlsx
@@ -500,7 +500,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8393" uniqueCount="1254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8401" uniqueCount="1255">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -4292,6 +4292,9 @@
   </si>
   <si>
     <t>050821003306</t>
+  </si>
+  <si>
+    <t>090821003319</t>
   </si>
 </sst>
 </file>
@@ -8598,10 +8601,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="13.375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="37.125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="20.125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="27.625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="37.125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18327,7 +18330,7 @@
         <v>106</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
     </row>
   </sheetData>
@@ -23334,7 +23337,7 @@
     <col min="6" max="46" customWidth="true" style="4" width="9.0" collapsed="true"/>
     <col min="47" max="47" customWidth="true" style="4" width="3.125" collapsed="true"/>
     <col min="48" max="59" style="4" width="9.0" collapsed="true"/>
-    <col min="60" max="60" style="4" width="9.0" collapsed="false"/>
+    <col min="60" max="60" style="4" width="9.0" collapsed="true"/>
     <col min="61" max="16384" style="4" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>